<commit_message>
análise de tweets finalizada
</commit_message>
<xml_diff>
--- a/iFood.xlsx
+++ b/iFood.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Área de Trabalho\Insper\Semestre 2\Ciencia de dados\P1\ciencia-dos-dados-p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA67D65B-5B4C-4F11-9505-96E9D515DA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45424830-9ABA-4F05-BB0A-988B4E07D0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2119,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B302" sqref="B302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3789,565 +3789,753 @@
       <c r="A208" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B208" s="6"/>
+      <c r="B208" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B209" s="6"/>
+      <c r="B209" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="210" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B210" s="6"/>
+      <c r="B210" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="211" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B211" s="6"/>
+      <c r="B211" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="212" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B212" s="6"/>
+      <c r="B212" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="213" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B213" s="6"/>
+      <c r="B213" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="214" spans="1:2" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B214" s="6"/>
+      <c r="B214" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="215" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B215" s="6"/>
+      <c r="B215" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="216" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B216" s="6"/>
+      <c r="B216" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="217" spans="1:2" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B217" s="6"/>
+      <c r="B217" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="218" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B218" s="6"/>
+      <c r="B218" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="219" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B219" s="6"/>
+      <c r="B219" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="220" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B220" s="6"/>
+      <c r="B220" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="221" spans="1:2" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B221" s="6"/>
+      <c r="B221" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="222" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B222" s="6"/>
+      <c r="B222" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="223" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B223" s="6"/>
+      <c r="B223" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="224" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B224" s="6"/>
+      <c r="B224" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B225" s="6"/>
+      <c r="B225" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="226" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A226" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B226" s="6"/>
+      <c r="B226" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="227" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B227" s="6"/>
+      <c r="B227" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="228" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B228" s="6"/>
+      <c r="B228" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="229" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B229" s="6"/>
+      <c r="B229" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="230" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B230" s="6"/>
+      <c r="B230" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B231" s="6"/>
+      <c r="B231" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="232" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B232" s="6"/>
+      <c r="B232" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="233" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B233" s="6"/>
+      <c r="B233" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A234" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B234" s="6"/>
+      <c r="B234" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="235" spans="1:2" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A235" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B235" s="6"/>
+      <c r="B235" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="236" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B236" s="6"/>
+      <c r="B236" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="237" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B237" s="6"/>
+      <c r="B237" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="238" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B238" s="6"/>
+      <c r="B238" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B239" s="6"/>
+      <c r="B239" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="240" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B240" s="6"/>
+      <c r="B240" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="241" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B241" s="6"/>
+      <c r="B241" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="242" spans="1:2" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B242" s="6"/>
+      <c r="B242" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="243" spans="1:2" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B243" s="6"/>
+      <c r="B243" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="244" spans="1:2" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A244" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B244" s="6"/>
+      <c r="B244" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B245" s="6"/>
+      <c r="B245" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="246" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B246" s="6"/>
+      <c r="B246" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B247" s="6"/>
+      <c r="B247" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="248" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B248" s="6"/>
+      <c r="B248" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="249" spans="1:2" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B249" s="6"/>
+      <c r="B249" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B250" s="6"/>
+      <c r="B250" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="6"/>
+      <c r="B251" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="252" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B252" s="6"/>
+      <c r="B252" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="253" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A253" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B253" s="6"/>
+      <c r="B253" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="254" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B254" s="6"/>
+      <c r="B254" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B255" s="6"/>
+      <c r="B255" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B256" s="6"/>
+      <c r="B256" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="257" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B257" s="6"/>
+      <c r="B257" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="258" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B258" s="6"/>
+      <c r="B258" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="259" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A259" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B259" s="6"/>
+      <c r="B259" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A260" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B260" s="6"/>
+      <c r="B260" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="261" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B261" s="6"/>
+      <c r="B261" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B262" s="6"/>
+      <c r="B262" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="263" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B263" s="6"/>
+      <c r="B263" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="264" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B264" s="6"/>
+      <c r="B264" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="265" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B265" s="6"/>
+      <c r="B265" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="266" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B266" s="6"/>
+      <c r="B266" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="267" spans="1:2" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B267" s="6"/>
+      <c r="B267" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="268" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B268" s="6"/>
+      <c r="B268" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="269" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B269" s="6"/>
+      <c r="B269" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="270" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B270" s="6"/>
+      <c r="B270" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B271" s="6"/>
+      <c r="B271" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="272" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B272" s="6"/>
+      <c r="B272" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="273" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A273" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B273" s="6"/>
+      <c r="B273" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="274" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B274" s="6"/>
+      <c r="B274" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="275" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A275" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B275" s="6"/>
+      <c r="B275" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="276" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B276" s="6"/>
+      <c r="B276" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="277" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A277" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B277" s="6"/>
+      <c r="B277" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="278" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A278" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B278" s="6"/>
+      <c r="B278" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="279" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A279" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B279" s="6"/>
+      <c r="B279" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="280" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A280" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B280" s="6"/>
+      <c r="B280" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="281" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B281" s="6"/>
+      <c r="B281" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="282" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A282" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B282" s="6"/>
+      <c r="B282" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="283" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A283" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B283" s="6"/>
+      <c r="B283" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="284" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A284" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B284" s="6"/>
+      <c r="B284" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="285" spans="1:2" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B285" s="6"/>
+      <c r="B285" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B286" s="6"/>
+      <c r="B286" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="287" spans="1:2" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A287" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B287" s="6"/>
+      <c r="B287" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B288" s="6"/>
+      <c r="B288" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="289" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A289" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B289" s="6"/>
+      <c r="B289" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="290" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A290" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B290" s="6"/>
+      <c r="B290" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="291" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B291" s="6"/>
+      <c r="B291" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="292" spans="1:2" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A292" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B292" s="6"/>
+      <c r="B292" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="293" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B293" s="6"/>
+      <c r="B293" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="294" spans="1:2" s="2" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A294" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B294" s="6"/>
+      <c r="B294" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="295" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A295" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B295" s="6"/>
+      <c r="B295" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="296" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A296" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B296" s="6"/>
+      <c r="B296" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="297" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A297" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B297" s="6"/>
+      <c r="B297" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="298" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A298" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B298" s="6"/>
+      <c r="B298" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="299" spans="1:2" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A299" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B299" s="6"/>
+      <c r="B299" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="300" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B300" s="6"/>
+      <c r="B300" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="301" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A301" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B301" s="6"/>
+      <c r="B301" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>